<commit_message>
finalizando V1 do programa
</commit_message>
<xml_diff>
--- a/musicas/musicas.xlsx
+++ b/musicas/musicas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrique\Documents\Programas\Shalom\Louvor-Shalom\musicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61712785-8361-4B44-A9D0-E0D059F04323}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEB28FF-3447-47D3-814A-6713B7731BB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{D26C8756-4B70-4E7D-9A2E-A034F97497FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D26C8756-4B70-4E7D-9A2E-A034F97497FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
-  <si>
-    <t>Musicas</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>Tom</t>
   </si>
@@ -91,6 +88,75 @@
   </si>
   <si>
     <t>Andamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eu me alegrarei </t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Edilson Botelho</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Ao único</t>
+  </si>
+  <si>
+    <t>Em</t>
+  </si>
+  <si>
+    <t>Ainda que a figueira</t>
+  </si>
+  <si>
+    <t>Fernandinho</t>
+  </si>
+  <si>
+    <t>Grandioso és tu</t>
+  </si>
+  <si>
+    <t>Hinário</t>
+  </si>
+  <si>
+    <t>André Valadão</t>
+  </si>
+  <si>
+    <t>Cantarei teu amor pra sempre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canção dos Filipenses </t>
+  </si>
+  <si>
+    <t>Comunid. da Vila</t>
+  </si>
+  <si>
+    <t>Bondade de Deus</t>
+  </si>
+  <si>
+    <t>Isaias Saad</t>
+  </si>
+  <si>
+    <t>Espírito, enche a minha vida - Ao Único</t>
+  </si>
+  <si>
+    <t>Eliana Ribeiro</t>
+  </si>
+  <si>
+    <t>Vineyard</t>
+  </si>
+  <si>
+    <t>Quebrantado</t>
+  </si>
+  <si>
+    <t>É de Coração</t>
+  </si>
+  <si>
+    <t>Paulo Cesar Baruk</t>
+  </si>
+  <si>
+    <t>Musica</t>
   </si>
 </sst>
 </file>
@@ -147,11 +213,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -475,205 +538,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711FD231-A939-43D3-A00D-FCFA7F85450B}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E17">

</xml_diff>

<commit_message>
Finalização da V1 do programa da shalom
</commit_message>
<xml_diff>
--- a/musicas/musicas.xlsx
+++ b/musicas/musicas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrique\Documents\Programas\Shalom\Louvor-Shalom\musicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEB28FF-3447-47D3-814A-6713B7731BB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC37F625-A6BE-45B5-B3DE-EE42EEF1F34A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D26C8756-4B70-4E7D-9A2E-A034F97497FF}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{D26C8756-4B70-4E7D-9A2E-A034F97497FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t>Tom</t>
   </si>
@@ -157,6 +157,60 @@
   </si>
   <si>
     <t>Musica</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7DH_tKN_n-g</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=4GC0uxYbJ-M</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=x1h5h1VWN6Y</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=K9wXc0FWITM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nv-T2_JPKZA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=JheqX_w3m08</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=BqzYurSgAtk</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=b0lQYSjyMfM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=60CuZyzGf5U</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1DzK7Wm3IcE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=oAyIGD3Ek7g</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=3JUS_ueGjnA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=KhVSYlfiL84</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=mZ9yZYo9Mmk</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cbAu_85RRtc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QbnmpJo3DiI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=5-srhflJ-kg</t>
   </si>
 </sst>
 </file>
@@ -213,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,6 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,22 +593,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711FD231-A939-43D3-A00D-FCFA7F85450B}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -569,8 +625,11 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -584,8 +643,11 @@
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -599,8 +661,11 @@
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -614,8 +679,11 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -629,8 +697,11 @@
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -644,8 +715,11 @@
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -659,8 +733,11 @@
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -674,8 +751,11 @@
       <c r="E8" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -689,8 +769,11 @@
       <c r="E9" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -704,8 +787,11 @@
       <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -719,8 +805,11 @@
       <c r="E11" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -734,8 +823,11 @@
       <c r="E12" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
@@ -749,8 +841,11 @@
       <c r="E13" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>33</v>
       </c>
@@ -764,8 +859,11 @@
       <c r="E14" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>35</v>
       </c>
@@ -779,8 +877,11 @@
       <c r="E15" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>37</v>
       </c>
@@ -794,8 +895,11 @@
       <c r="E16" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
@@ -809,8 +913,11 @@
       <c r="E17" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>41</v>
       </c>
@@ -823,6 +930,9 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
         <v>42</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>